<commit_message>
Se arregló Tablero con los tiempo
</commit_message>
<xml_diff>
--- a/Tablero.xlsx
+++ b/Tablero.xlsx
@@ -49,32 +49,23 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFDBBD"/>
+        <fgColor rgb="FFB53430"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB53430"/>
+        <fgColor rgb="FFFFDBBD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
+  <borders count="16">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -82,9 +73,7 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -93,26 +82,12 @@
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -121,9 +96,7 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -134,7 +107,9 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -142,29 +117,27 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
@@ -178,32 +151,126 @@
       <diagonal style="medium">
         <color auto="1"/>
       </diagonal>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,73 +565,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C4:J9"/>
+  <dimension ref="C4:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="4" spans="3:10">
+    <row r="4" spans="3:9">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="3:10">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="9"/>
+    <row r="5" spans="3:9">
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="3:10">
-      <c r="C6" s="10"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="3"/>
+    <row r="6" spans="3:9">
+      <c r="C6" s="11"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="3:10">
-      <c r="C7" s="7"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="9"/>
+    <row r="7" spans="3:9">
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="3:10">
-      <c r="C8" s="3"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="6"/>
+    <row r="8" spans="3:9">
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="3:10">
-      <c r="C9" s="17"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+    <row r="9" spans="3:9">
+      <c r="C9" s="7"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="7"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="3:9">
+      <c r="C10" s="23"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>